<commit_message>
Created code to take screenshot
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/data.xlsx
+++ b/src/test/java/TestData/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nkosi/Projects/Automation2025/firstGroup2025/src/test/java/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73E3521-80C2-9E4E-BA17-4D1A241C4410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54BB94A-5DCA-E04B-9FDB-C166B9CEA856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="2660" windowWidth="33600" windowHeight="18940" xr2:uid="{B8A52318-12D5-3B46-8F7E-8A17FF9AA0D3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
   <si>
     <t>Password</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>Cele</t>
-  </si>
-  <si>
-    <t>standard_userNkosi</t>
   </si>
 </sst>
 </file>
@@ -502,7 +499,7 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,7 +518,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>

</xml_diff>